<commit_message>
some firmware server bugs; work on simulator
</commit_message>
<xml_diff>
--- a/model_params.xlsx
+++ b/model_params.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="644" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Parameters" sheetId="1" state="visible" r:id="rId2"/>
@@ -15,811 +15,816 @@
     <sheet name="sao_spec" sheetId="5" state="visible" r:id="rId6"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <extLst>
+    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
+      <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="784" uniqueCount="267">
   <si>
-    <t>key</t>
-  </si>
-  <si>
-    <t>bitstream</t>
-  </si>
-  <si>
-    <t>date</t>
-  </si>
-  <si>
-    <t>nchans</t>
-  </si>
-  <si>
-    <t>n_par_streams</t>
-  </si>
-  <si>
-    <t>interleaved</t>
-  </si>
-  <si>
-    <t>design bandwidth</t>
-  </si>
-  <si>
-    <t>desired_rf_level</t>
-  </si>
-  <si>
-    <t>adc_type</t>
-  </si>
-  <si>
-    <t>ADC inputs</t>
-  </si>
-  <si>
-    <t>spectrum_bits</t>
-  </si>
-  <si>
-    <t>fft_shift</t>
-  </si>
-  <si>
-    <t>gbe0 MAC</t>
-  </si>
-  <si>
-    <t>gbe0 IP</t>
-  </si>
-  <si>
-    <t>gbe1 MAC</t>
-  </si>
-  <si>
-    <t>gbe1 IP</t>
-  </si>
-  <si>
-    <t>gbe2 MAC</t>
-  </si>
-  <si>
-    <t>gbe2 IP</t>
-  </si>
-  <si>
-    <t>gbe3 MAC</t>
-  </si>
-  <si>
-    <t>gbe3 IP</t>
-  </si>
-  <si>
-    <t>hires_spec</t>
-  </si>
-  <si>
-    <t>r_spec_1ghz_16k_kadc_r110.bof</t>
-  </si>
-  <si>
-    <t>katadc</t>
-  </si>
-  <si>
-    <t>0,;,</t>
-  </si>
-  <si>
-    <t>sao_spec</t>
-  </si>
-  <si>
-    <t>tams32k_dave_2014_Jul_01_1504.bof</t>
-  </si>
-  <si>
-    <t>kurt_spec</t>
-  </si>
-  <si>
-    <t>dsn_gains_v1_2015_Feb_05_1455.bof</t>
-  </si>
-  <si>
-    <t>0,1;,</t>
-  </si>
-  <si>
-    <t>00:12:34:56:78:99</t>
-  </si>
-  <si>
-    <t>10.0.0.1</t>
-  </si>
-  <si>
-    <t>kurt_spec-2</t>
-  </si>
-  <si>
-    <t>dsn_spec_10ge_v6_2014_Apr_14_1432.bof</t>
-  </si>
-  <si>
-    <t>Register</t>
-  </si>
-  <si>
-    <t>Dir</t>
-  </si>
-  <si>
-    <t>Bits</t>
-  </si>
-  <si>
-    <t>sub_name</t>
-  </si>
-  <si>
-    <t>purpose</t>
-  </si>
-  <si>
-    <t>value</t>
-  </si>
-  <si>
-    <t>notes</t>
-  </si>
-  <si>
-    <t>acc_cnt</t>
-  </si>
-  <si>
-    <t>R</t>
-  </si>
-  <si>
-    <t>31:0</t>
-  </si>
-  <si>
-    <t>counts the number of accumulations.</t>
-  </si>
-  <si>
-    <t>Can be reset by “control” register bit[1].</t>
-  </si>
-  <si>
-    <t>acc_len</t>
-  </si>
-  <si>
-    <t>R/W</t>
-  </si>
-  <si>
-    <t>number of spectra to be accumulated</t>
-  </si>
-  <si>
-    <t>adc_ctrl0</t>
-  </si>
-  <si>
-    <t>W</t>
-  </si>
-  <si>
-    <t>rf_enable</t>
-  </si>
-  <si>
-    <t>KATADC RF section enable</t>
-  </si>
-  <si>
-    <t>5:0</t>
-  </si>
-  <si>
-    <t>atten</t>
-  </si>
-  <si>
-    <t>attenuation</t>
-  </si>
-  <si>
-    <t>0-63</t>
-  </si>
-  <si>
-    <t>0-31.5 dB in 0.5 dB steps</t>
-  </si>
-  <si>
-    <t>adc_sum_sq0</t>
-  </si>
-  <si>
-    <t>sum of the squares of 65536 ADC samples</t>
-  </si>
-  <si>
-    <t>control</t>
-  </si>
-  <si>
-    <t>adc_protect_disable</t>
-  </si>
-  <si>
-    <t>disable ADC overload protection</t>
-  </si>
-  <si>
-    <t>flasher_en</t>
-  </si>
-  <si>
-    <t>clr_status</t>
-  </si>
-  <si>
-    <t>cnt_rst</t>
-  </si>
-  <si>
-    <t>pulse high to clear all counters</t>
-  </si>
-  <si>
-    <t>mrst</t>
-  </si>
-  <si>
-    <t>resets gbe0 and acc_cnt</t>
-  </si>
-  <si>
-    <t>duty_cnt</t>
-  </si>
-  <si>
-    <t>duty_period</t>
-  </si>
-  <si>
-    <t>shifting schedule to prevent FFT overflow</t>
-  </si>
-  <si>
-    <t>Bit 0 specifies the behavior of stage 0, bit 1 of stage 1, and so on. If a stage is set to shift (with bit = 1), then every sample is divided by 2 at the output of that stage.</t>
-  </si>
-  <si>
-    <t>iic_adc0</t>
-  </si>
-  <si>
-    <t>256*[7:0]</t>
-  </si>
-  <si>
-    <t>internal I2C registers for the KATADC.</t>
-  </si>
-  <si>
-    <t>kat_adc_controller</t>
-  </si>
-  <si>
-    <t>4096*[7:0]</t>
-  </si>
-  <si>
-    <t>Built-in register for KATADC block instantiation.</t>
-  </si>
-  <si>
-    <t>For monitoring and debugging purposes.</t>
-  </si>
-  <si>
-    <t>snap_adc_bram</t>
-  </si>
-  <si>
-    <t>16384*7:0</t>
-  </si>
-  <si>
-    <t>ADC samples snapshot</t>
-  </si>
-  <si>
-    <t>snap_adc_ctrl</t>
-  </si>
-  <si>
-    <t>snap_adc_status</t>
-  </si>
-  <si>
-    <t>snap_adc_tr_en_cnt</t>
-  </si>
-  <si>
-    <t>snap_adc_trig_offset</t>
-  </si>
-  <si>
-    <t>status</t>
-  </si>
-  <si>
-    <t>fft_overrange</t>
-  </si>
-  <si>
-    <t>FFT over-range latch</t>
-  </si>
-  <si>
-    <t>fft_bad</t>
-  </si>
-  <si>
-    <t>ADC over-range latch</t>
-  </si>
-  <si>
-    <t>adc_bad</t>
-  </si>
-  <si>
-    <t>ADC bad latch</t>
-  </si>
-  <si>
-    <t>mean square value exceeds threshold, ADC is disabled unless overridden by control [13]</t>
-  </si>
-  <si>
-    <t>store0</t>
-  </si>
-  <si>
-    <t>32768*7:0</t>
-  </si>
-  <si>
-    <t>store1</t>
-  </si>
-  <si>
-    <t>store2</t>
-  </si>
-  <si>
-    <t>store3</t>
-  </si>
-  <si>
-    <t>sync_cnt</t>
-  </si>
-  <si>
-    <t>Counts number of sync pulses generated my an internal counter.</t>
-  </si>
-  <si>
-    <t>Will be removed in future firmware revision.</t>
-  </si>
-  <si>
-    <t>sys_board_id</t>
-  </si>
-  <si>
-    <t>Static system register</t>
-  </si>
-  <si>
-    <t>sys_clkcounter</t>
-  </si>
-  <si>
-    <t>Counts number of clocks that runs the logic.</t>
-  </si>
-  <si>
-    <t>sys_rev</t>
-  </si>
-  <si>
-    <t>Static system register.</t>
-  </si>
-  <si>
-    <t>sys_rev_rcs</t>
-  </si>
-  <si>
-    <t>sys_scratchpad</t>
-  </si>
-  <si>
-    <t>Test register</t>
-  </si>
-  <si>
-    <t>See if accesses across the bus are OK. (Timing issues, etc. can make this a problem.)</t>
-  </si>
-  <si>
-    <t>trig_level</t>
-  </si>
-  <si>
-    <t>bits</t>
-  </si>
-  <si>
-    <t>acc_len_m1</t>
-  </si>
-  <si>
-    <t>Sets the accumulation length.</t>
-  </si>
-  <si>
-    <t>1...63</t>
-  </si>
-  <si>
-    <t>Value must be one smaller than desired length. Maximum length: 64.  Setting register to '0' not supported for normal use</t>
-  </si>
-  <si>
-    <t>adc_atten</t>
-  </si>
-  <si>
-    <t>rf0</t>
-  </si>
-  <si>
-    <t>11:6</t>
-  </si>
-  <si>
-    <t>rf1</t>
-  </si>
-  <si>
-    <t>64-4095</t>
-  </si>
-  <si>
-    <t>adc_en</t>
-  </si>
-  <si>
-    <t>0</t>
-  </si>
-  <si>
-    <t>Enables the RF section</t>
-  </si>
-  <si>
-    <t>0-1</t>
-  </si>
-  <si>
-    <t>adc_snap_trig</t>
-  </si>
-  <si>
-    <t>pol0_snap_trig</t>
-  </si>
-  <si>
-    <t>initiates collection of raw ADC data for pol0 only (rising edge)</t>
-  </si>
-  <si>
-    <t>pol1_snap_trig</t>
-  </si>
-  <si>
-    <t>initiates collection of raw ADC data for pol1 only (rising edge)</t>
-  </si>
-  <si>
-    <t>initiates collection of raw ADC data for both pols simultaneously</t>
-  </si>
-  <si>
-    <t>allow_all_spectra</t>
-  </si>
-  <si>
-    <t>Controls the python output interface.</t>
-  </si>
-  <si>
-    <t>Always set to '1' for normal operation</t>
-  </si>
-  <si>
-    <t>allow_next_spectrum_posedge</t>
-  </si>
-  <si>
-    <t>Always set to '0' for normal operation</t>
-  </si>
-  <si>
-    <t>bit_select_counter_out</t>
-  </si>
-  <si>
-    <t>Controls data input to 10GbE block.</t>
-  </si>
-  <si>
-    <t>Data routed from DSP</t>
-  </si>
-  <si>
-    <t>data routed from bank of counters for testing purposes</t>
-  </si>
-  <si>
-    <t>14</t>
-  </si>
-  <si>
-    <t>dsp_reset_hits_tge</t>
-  </si>
-  <si>
-    <t>Controls reset source for 10GbE block</t>
-  </si>
-  <si>
-    <t>10GbE block reset only by 'sys_rst'</t>
-  </si>
-  <si>
-    <t>10GbE block reset by 'sys_rst' OR dsp reset</t>
-  </si>
-  <si>
-    <t>13</t>
-  </si>
-  <si>
-    <t>12</t>
-  </si>
-  <si>
-    <t>3</t>
-  </si>
-  <si>
-    <t>level high: reset 'gbe0_tx_cnt' counter</t>
-  </si>
-  <si>
-    <t>sys_rst</t>
-  </si>
-  <si>
-    <t>Resets 10GbE block</t>
-  </si>
-  <si>
-    <t>dest_ip</t>
-  </si>
-  <si>
-    <t>IP for sending packets through 10GbE</t>
-  </si>
-  <si>
-    <t>dest_port</t>
-  </si>
-  <si>
-    <t>15:0</t>
-  </si>
-  <si>
-    <t>Port for sending packets for pol1</t>
-  </si>
-  <si>
-    <t>31:16</t>
-  </si>
-  <si>
-    <t>Port for sending packets for pol0</t>
-  </si>
-  <si>
-    <t>gbe0</t>
-  </si>
-  <si>
-    <t>gbe0_linkup</t>
-  </si>
-  <si>
-    <t>True if CX4-0 is connected to a network. Tied to 'led_up' port of 10GbE port</t>
-  </si>
-  <si>
-    <t>gbe0_rx</t>
-  </si>
-  <si>
-    <t>True if the block is receiving data; tied to 'led_rx' port of 10GbE port</t>
-  </si>
-  <si>
-    <t>gbe0_tx</t>
-  </si>
-  <si>
-    <t>True if the block is transmitting data; tied to 'led_tx' port of 10GbE port</t>
-  </si>
-  <si>
-    <t>gbe0_tx_cnt</t>
-  </si>
-  <si>
-    <t>Counts the number of frames transmitted during a packet.</t>
-  </si>
-  <si>
-    <t>gbe0_tx_full</t>
-  </si>
-  <si>
-    <t>True if FIFO is almost full; tied to 'tx_full' port of 10GbE port (connected to negedge block, may be always '0')</t>
-  </si>
-  <si>
-    <t>gbe0_tx_over</t>
-  </si>
-  <si>
-    <t>True if FIFO has overflowed and data were lost; tied to 'tx_overflow' port of 10GbE port (connected to negedge block, may be always '0')</t>
-  </si>
-  <si>
-    <t>one_pps_mask</t>
-  </si>
-  <si>
-    <t>3:0</t>
-  </si>
-  <si>
-    <t>masks the 1pps signal, so that it can only be received by a subset of the four 1pps inputs</t>
-  </si>
-  <si>
-    <t>0b0000</t>
-  </si>
-  <si>
-    <t>Bit=0: 1pps disabled for this simultaneous input</t>
-  </si>
-  <si>
-    <t>0bXXXX</t>
-  </si>
-  <si>
-    <t>Bit=1: 1pps enabled for this simultaneous input</t>
-  </si>
-  <si>
-    <t>out_fourth_lower</t>
-  </si>
-  <si>
-    <t>512*31:0</t>
-  </si>
-  <si>
-    <t>Kurtosis data for pol0, channels 0:511</t>
-  </si>
-  <si>
-    <t>Contains kurtosis data for outputs of accumulations.  Divide values by 2^24 to receive actual values (make sure to floating point divide)</t>
-  </si>
-  <si>
-    <t>out_fourth_lower_1</t>
-  </si>
-  <si>
-    <t>Kurtosis data for pol0, channels 512:1023</t>
-  </si>
-  <si>
-    <t>out_fourth_lower_2</t>
-  </si>
-  <si>
-    <t>Kurtosis data for pol1, channels 0:511</t>
-  </si>
-  <si>
-    <t>out_fourth_lower_3</t>
-  </si>
-  <si>
-    <t>Kurtosis data for pol1, channels 512:1023</t>
-  </si>
-  <si>
-    <t>out_pow_lower_0</t>
-  </si>
-  <si>
-    <t>Power data for pol0, channels 0:511</t>
-  </si>
-  <si>
-    <t>Contains power data for outputs of accumulations.  Arbitrary units, affected by bit selection.</t>
-  </si>
-  <si>
-    <t>out_pow_lower_1</t>
-  </si>
-  <si>
-    <t>Power data for pol0, channels 512:1023</t>
-  </si>
-  <si>
-    <t>out_pow_lower_2</t>
-  </si>
-  <si>
-    <t>Power data for pol1, channels 0:511</t>
-  </si>
-  <si>
-    <t>out_pow_lower_3</t>
-  </si>
-  <si>
-    <t>Power data for pol1, channels 512:1023</t>
-  </si>
-  <si>
-    <t>pkt_header_upper</t>
-  </si>
-  <si>
-    <t>Controls the upper 32 bits of the 10GbE header's user-controlled segment</t>
-  </si>
-  <si>
-    <t>pkt_header_lower</t>
-  </si>
-  <si>
-    <t>Controls the lower 32 bits of the 10GbE header's user-controlled segment</t>
-  </si>
-  <si>
-    <t>pkt_cnt_sec_rst_ctrl</t>
-  </si>
-  <si>
-    <t>Selects the reset source for the 'pkt_cnt_sec' counter, which is the number of the packet in the current second.</t>
-  </si>
-  <si>
-    <t>reset by DSP sync input</t>
-  </si>
-  <si>
-    <t>reset by 1pps input (per masking by one_pps_mask)</t>
-  </si>
-  <si>
-    <t>raw_pkt_cnt_out</t>
-  </si>
-  <si>
-    <t>Either number of packets sent or FPGA clock ticks</t>
-  </si>
-  <si>
-    <t>raw_pkt_cnt_is_fpga_clocks</t>
-  </si>
-  <si>
-    <t>Controls what datum is in raw_pkt_cnt_out</t>
-  </si>
-  <si>
-    <t>raw_pkt_cnt increments upon completion of each packet</t>
-  </si>
-  <si>
-    <t>raw_pkt_cnt increments every FPGA clock cycle</t>
-  </si>
-  <si>
-    <t>raw_pkt_cnt_rst_ctrl</t>
-  </si>
-  <si>
-    <t>1:0</t>
-  </si>
-  <si>
-    <t>Selects the reset source for the 'raw_pkt_cnt' counter</t>
-  </si>
-  <si>
-    <t>reset by 'raw_pkt_cnt_rst_mine'</t>
-  </si>
-  <si>
-    <t>raw_pkt_cnt_rst_mine</t>
-  </si>
-  <si>
-    <t>(raw_pkt_cnt_rst_ctrl != 2): no effect; (raw_pkt_cnt_rst_ctrl == 2): level high resets 'raw_pkt_cnt' register</t>
-  </si>
-  <si>
-    <t>sec_cnt_rst</t>
-  </si>
-  <si>
-    <t>Resets the 'sec_cnt' counter. 'sec_cnt' is written to the header of each packet.</t>
-  </si>
-  <si>
-    <t>Level high (counter remains at '0' while register = '1') (reset is level high)</t>
-  </si>
-  <si>
-    <t>select_bits_pow</t>
-  </si>
-  <si>
-    <t>4:0</t>
-  </si>
-  <si>
-    <t>Selects which 16 bits of the accumulated power vector to send to the 10GbE.</t>
-  </si>
-  <si>
-    <t>A value of '5' represents the 16 most significant bits, where each incremental larger value moves the window down by one bit, towards the LSB.</t>
-  </si>
-  <si>
-    <t>snap_raw_pol0_addr</t>
-  </si>
-  <si>
-    <t>~11:0</t>
-  </si>
-  <si>
-    <t>ignore, no meaningful use</t>
-  </si>
-  <si>
-    <t>snap_raw_pol0_bram</t>
-  </si>
-  <si>
-    <t>2048*31:0</t>
-  </si>
-  <si>
-    <t>contains raw ADC data(pol0), one sample per byte</t>
-  </si>
-  <si>
-    <t>snap_raw_pol0_ctrl</t>
-  </si>
-  <si>
-    <t>standard SNAP control interface</t>
-  </si>
-  <si>
-    <t>snap_raw_pol1_addr</t>
-  </si>
-  <si>
-    <t>snap_raw_pol1_bram</t>
-  </si>
-  <si>
-    <t>contains raw ADC data(pol1), one sample per byte</t>
-  </si>
-  <si>
-    <t>snap_raw_pol1_ctrl</t>
-  </si>
-  <si>
-    <t>snap64_tge_addr</t>
-  </si>
-  <si>
-    <t>snap64_tge_bram_lsb</t>
-  </si>
-  <si>
-    <t>contains upper 32 bits per cycle of 10 GbE packet data</t>
-  </si>
-  <si>
-    <t>snap64_tge_bram_msb</t>
-  </si>
-  <si>
-    <t>contains lower 32 bits per cycle of 10 GbE packet data</t>
-  </si>
-  <si>
-    <t>snap64_tge_ctrl</t>
-  </si>
-  <si>
-    <t>spec2_delay</t>
-  </si>
-  <si>
-    <t>spec2_en</t>
-  </si>
-  <si>
-    <t>spec_count</t>
-  </si>
-  <si>
-    <t>Counts spectra</t>
-  </si>
-  <si>
-    <t>Increments for each spectrum accumulation which has finished.  Resets on DSP reset.</t>
-  </si>
-  <si>
-    <t>sync_in</t>
-  </si>
-  <si>
-    <t>Software synch pulse</t>
-  </si>
-  <si>
-    <t>Sync provided by rising edge of 1pps if sync_sel_in = 1</t>
-  </si>
-  <si>
-    <t>sync_in_sel</t>
-  </si>
-  <si>
-    <t>Selects the input sync pulse to the DSP</t>
-  </si>
-  <si>
-    <t>Sync provided by rising edge of 'sync_in' register</t>
-  </si>
-  <si>
-    <t>Sync provided by rising edge of 1pps</t>
-  </si>
-  <si>
-    <t>out_fourth_lower_0</t>
-  </si>
-  <si>
-    <t>Is incremented for every clock cycle when the square of the ADC values is greater than the trig_level squared.</t>
-  </si>
-  <si>
-    <t>Resets duty_cnt every duty_period number of clock cycles</t>
-  </si>
-  <si>
-    <t>Bit 31 is high while the buffer is being filled. Bits 30:0 have the address of the byte currently being written.</t>
-  </si>
-  <si>
-    <t>Counts number of sync pulses generated by an internal counter.</t>
-  </si>
-  <si>
-    <t>sync_start</t>
-  </si>
-  <si>
-    <t>synchronize the inputs of the different FFTs to a single clock</t>
-  </si>
-  <si>
-    <t>0/1</t>
-  </si>
-  <si>
-    <t>Toggle in 0/1/0 sequence.</t>
-  </si>
-  <si>
-    <t>cycle.</t>
-  </si>
-  <si>
-    <t>trig_level value is squared, and compared to the square of the ADC values. If the square of the ADC values is greater, it triggers data capture to the "snap_adc" block.</t>
+    <t xml:space="preserve">key</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bitstream</t>
+  </si>
+  <si>
+    <t xml:space="preserve">date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nchans</t>
+  </si>
+  <si>
+    <t xml:space="preserve">n_par_streams</t>
+  </si>
+  <si>
+    <t xml:space="preserve">interleaved</t>
+  </si>
+  <si>
+    <t xml:space="preserve">design bandwidth</t>
+  </si>
+  <si>
+    <t xml:space="preserve">desired_rf_level</t>
+  </si>
+  <si>
+    <t xml:space="preserve">adc_type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ADC inputs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">spectrum_bits</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fft_shift</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gbe0 MAC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gbe0 IP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gbe1 MAC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gbe1 IP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gbe2 MAC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gbe2 IP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gbe3 MAC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gbe3 IP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hires_spec</t>
+  </si>
+  <si>
+    <t xml:space="preserve">r_spec_1ghz_16k_kadc_r110.bof</t>
+  </si>
+  <si>
+    <t xml:space="preserve">katadc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0,;,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sao_spec</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tams32k_dave_2014_Jul_01_1504.bof</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kurt_spec</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dsn_gains_v1_2015_Feb_05_1455.bof</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0,1;,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">00:12:34:56:78:99</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10.0.0.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kurt_spec-2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dsn_spec_10ge_v6_2014_Apr_14_1432.bof</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Register</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dir</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bits</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sub_name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">purpose</t>
+  </si>
+  <si>
+    <t xml:space="preserve">value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">notes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">acc_cnt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R</t>
+  </si>
+  <si>
+    <t xml:space="preserve">31:0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">counts the number of accumulations.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Can be reset by “control” register bit[1].</t>
+  </si>
+  <si>
+    <t xml:space="preserve">acc_len</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R/W</t>
+  </si>
+  <si>
+    <t xml:space="preserve">number of spectra to be accumulated</t>
+  </si>
+  <si>
+    <t xml:space="preserve">adc_ctrl0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">W</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rf_enable</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KATADC RF section enable</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5:0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">atten</t>
+  </si>
+  <si>
+    <t xml:space="preserve">attenuation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0-63</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0-31.5 dB in 0.5 dB steps</t>
+  </si>
+  <si>
+    <t xml:space="preserve">adc_sum_sq0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sum of the squares of 65536 ADC samples</t>
+  </si>
+  <si>
+    <t xml:space="preserve">control</t>
+  </si>
+  <si>
+    <t xml:space="preserve">adc_protect_disable</t>
+  </si>
+  <si>
+    <t xml:space="preserve">disable ADC overload protection</t>
+  </si>
+  <si>
+    <t xml:space="preserve">flasher_en</t>
+  </si>
+  <si>
+    <t xml:space="preserve">clr_status</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cnt_rst</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pulse high to clear all counters</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mrst</t>
+  </si>
+  <si>
+    <t xml:space="preserve">resets gbe0 and acc_cnt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">duty_cnt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">duty_period</t>
+  </si>
+  <si>
+    <t xml:space="preserve">shifting schedule to prevent FFT overflow</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bit 0 specifies the behavior of stage 0, bit 1 of stage 1, and so on. If a stage is set to shift (with bit = 1), then every sample is divided by 2 at the output of that stage.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">iic_adc0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">256*[7:0]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">internal I2C registers for the KATADC.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kat_adc_controller</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4096*[7:0]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Built-in register for KATADC block instantiation.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">For monitoring and debugging purposes.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">snap_adc_bram</t>
+  </si>
+  <si>
+    <t xml:space="preserve">16384*7:0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ADC samples snapshot</t>
+  </si>
+  <si>
+    <t xml:space="preserve">snap_adc_ctrl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">snap_adc_status</t>
+  </si>
+  <si>
+    <t xml:space="preserve">snap_adc_tr_en_cnt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">snap_adc_trig_offset</t>
+  </si>
+  <si>
+    <t xml:space="preserve">status</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fft_overrange</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FFT over-range latch</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fft_bad</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ADC over-range latch</t>
+  </si>
+  <si>
+    <t xml:space="preserve">adc_bad</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ADC bad latch</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mean square value exceeds threshold, ADC is disabled unless overridden by control [13]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">store0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">32768*7:0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">store1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">store2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">store3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sync_cnt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Counts number of sync pulses generated my an internal counter.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Will be removed in future firmware revision.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sys_board_id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Static system register</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sys_clkcounter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Counts number of clocks that runs the logic.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sys_rev</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Static system register.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sys_rev_rcs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sys_scratchpad</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test register</t>
+  </si>
+  <si>
+    <t xml:space="preserve">See if accesses across the bus are OK. (Timing issues, etc. can make this a problem.)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">trig_level</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bits</t>
+  </si>
+  <si>
+    <t xml:space="preserve">acc_len_m1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sets the accumulation length.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1...63</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Value must be one smaller than desired length. Maximum length: 64.  Setting register to '0' not supported for normal use</t>
+  </si>
+  <si>
+    <t xml:space="preserve">adc_atten</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rf0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11:6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rf1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">64-4095</t>
+  </si>
+  <si>
+    <t xml:space="preserve">adc_en</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Enables the RF section</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0-1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">adc_snap_trig</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pol0_snap_trig</t>
+  </si>
+  <si>
+    <t xml:space="preserve">initiates collection of raw ADC data for pol0 only (rising edge)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pol1_snap_trig</t>
+  </si>
+  <si>
+    <t xml:space="preserve">initiates collection of raw ADC data for pol1 only (rising edge)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">initiates collection of raw ADC data for both pols simultaneously</t>
+  </si>
+  <si>
+    <t xml:space="preserve">allow_all_spectra</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Controls the python output interface.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Always set to '1' for normal operation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">allow_next_spectrum_posedge</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Always set to '0' for normal operation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bit_select_counter_out</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Controls data input to 10GbE block.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Data routed from DSP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">data routed from bank of counters for testing purposes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dsp_reset_hits_tge</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Controls reset source for 10GbE block</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10GbE block reset only by 'sys_rst'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10GbE block reset by 'sys_rst' OR dsp reset</t>
+  </si>
+  <si>
+    <t xml:space="preserve">13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">level high: reset 'gbe0_tx_cnt' counter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sys_rst</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Resets 10GbE block</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dest_ip</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IP for sending packets through 10GbE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dest_port</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15:0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Port for sending packets for pol1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">31:16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Port for sending packets for pol0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gbe0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gbe0_linkup</t>
+  </si>
+  <si>
+    <t xml:space="preserve">True if CX4-0 is connected to a network. Tied to 'led_up' port of 10GbE port</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gbe0_rx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">True if the block is receiving data; tied to 'led_rx' port of 10GbE port</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gbe0_tx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">True if the block is transmitting data; tied to 'led_tx' port of 10GbE port</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gbe0_tx_cnt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Counts the number of frames transmitted during a packet.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gbe0_tx_full</t>
+  </si>
+  <si>
+    <t xml:space="preserve">True if FIFO is almost full; tied to 'tx_full' port of 10GbE port (connected to negedge block, may be always '0')</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gbe0_tx_over</t>
+  </si>
+  <si>
+    <t xml:space="preserve">True if FIFO has overflowed and data were lost; tied to 'tx_overflow' port of 10GbE port (connected to negedge block, may be always '0')</t>
+  </si>
+  <si>
+    <t xml:space="preserve">one_pps_mask</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3:0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">masks the 1pps signal, so that it can only be received by a subset of the four 1pps inputs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0b0000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bit=0: 1pps disabled for this simultaneous input</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0bXXXX</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bit=1: 1pps enabled for this simultaneous input</t>
+  </si>
+  <si>
+    <t xml:space="preserve">out_fourth_lower</t>
+  </si>
+  <si>
+    <t xml:space="preserve">512*31:0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kurtosis data for pol0, channels 0:511</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Contains kurtosis data for outputs of accumulations.  Divide values by 2^24 to receive actual values (make sure to floating point divide)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">out_fourth_lower_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kurtosis data for pol0, channels 512:1023</t>
+  </si>
+  <si>
+    <t xml:space="preserve">out_fourth_lower_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kurtosis data for pol1, channels 0:511</t>
+  </si>
+  <si>
+    <t xml:space="preserve">out_fourth_lower_3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kurtosis data for pol1, channels 512:1023</t>
+  </si>
+  <si>
+    <t xml:space="preserve">out_pow_lower_0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Power data for pol0, channels 0:511</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Contains power data for outputs of accumulations.  Arbitrary units, affected by bit selection.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">out_pow_lower_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Power data for pol0, channels 512:1023</t>
+  </si>
+  <si>
+    <t xml:space="preserve">out_pow_lower_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Power data for pol1, channels 0:511</t>
+  </si>
+  <si>
+    <t xml:space="preserve">out_pow_lower_3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Power data for pol1, channels 512:1023</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pkt_header_upper</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Controls the upper 32 bits of the 10GbE header's user-controlled segment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pkt_header_lower</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Controls the lower 32 bits of the 10GbE header's user-controlled segment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pkt_cnt_sec_rst_ctrl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Selects the reset source for the 'pkt_cnt_sec' counter, which is the number of the packet in the current second.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">reset by DSP sync input</t>
+  </si>
+  <si>
+    <t xml:space="preserve">reset by 1pps input (per masking by one_pps_mask)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">raw_pkt_cnt_out</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Either number of packets sent or FPGA clock ticks</t>
+  </si>
+  <si>
+    <t xml:space="preserve">raw_pkt_cnt_is_fpga_clocks</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Controls what datum is in raw_pkt_cnt_out</t>
+  </si>
+  <si>
+    <t xml:space="preserve">raw_pkt_cnt increments upon completion of each packet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">raw_pkt_cnt increments every FPGA clock cycle</t>
+  </si>
+  <si>
+    <t xml:space="preserve">raw_pkt_cnt_rst_ctrl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1:0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Selects the reset source for the 'raw_pkt_cnt' counter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">reset by 'raw_pkt_cnt_rst_mine'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">raw_pkt_cnt_rst_mine</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(raw_pkt_cnt_rst_ctrl != 2): no effect; (raw_pkt_cnt_rst_ctrl == 2): level high resets 'raw_pkt_cnt' register</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sec_cnt_rst</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Resets the 'sec_cnt' counter. 'sec_cnt' is written to the header of each packet.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Level high (counter remains at '0' while register = '1') (reset is level high)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">select_bits_pow</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4:0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Selects which 16 bits of the accumulated power vector to send to the 10GbE.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A value of '5' represents the 16 most significant bits, where each incremental larger value moves the window down by one bit, towards the LSB.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">snap_raw_pol0_addr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">~11:0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ignore, no meaningful use</t>
+  </si>
+  <si>
+    <t xml:space="preserve">snap_raw_pol0_bram</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2048*31:0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">contains raw ADC data(pol0), one sample per byte</t>
+  </si>
+  <si>
+    <t xml:space="preserve">snap_raw_pol0_ctrl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">standard SNAP control interface</t>
+  </si>
+  <si>
+    <t xml:space="preserve">snap_raw_pol1_addr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">snap_raw_pol1_bram</t>
+  </si>
+  <si>
+    <t xml:space="preserve">contains raw ADC data(pol1), one sample per byte</t>
+  </si>
+  <si>
+    <t xml:space="preserve">snap_raw_pol1_ctrl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">snap64_tge_addr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">snap64_tge_bram_lsb</t>
+  </si>
+  <si>
+    <t xml:space="preserve">contains upper 32 bits per cycle of 10 GbE packet data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">snap64_tge_bram_msb</t>
+  </si>
+  <si>
+    <t xml:space="preserve">contains lower 32 bits per cycle of 10 GbE packet data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">snap64_tge_ctrl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">spec2_delay</t>
+  </si>
+  <si>
+    <t xml:space="preserve">spec2_en</t>
+  </si>
+  <si>
+    <t xml:space="preserve">spec_count</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Counts spectra</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Increments for each spectrum accumulation which has finished.  Resets on DSP reset.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sync_in</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Software synch pulse</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sync provided by rising edge of 1pps if sync_sel_in = 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sync_in_sel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Selects the input sync pulse to the DSP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sync provided by rising edge of 'sync_in' register</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sync provided by rising edge of 1pps</t>
+  </si>
+  <si>
+    <t xml:space="preserve">out_fourth_lower_0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Is incremented for every clock cycle when the square of the ADC values is greater than the trig_level squared.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Resets duty_cnt every duty_period number of clock cycles</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bit 31 is high while the buffer is being filled. Bits 30:0 have the address of the byte currently being written.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Counts number of sync pulses generated by an internal counter.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sync_start</t>
+  </si>
+  <si>
+    <t xml:space="preserve">synchronize the inputs of the different FFTs to a single clock</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0/1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Toggle in 0/1/0 sequence.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cycle.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">trig_level value is squared, and compared to the square of the ADC values. If the square of the ADC values is greater, it triggers data capture to the "snap_adc" block.</t>
   </si>
 </sst>
 </file>
@@ -827,7 +832,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="164" formatCode="GENERAL"/>
+    <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
     <numFmt numFmtId="166" formatCode="YYYY\ MMM\ D\ HH:MM"/>
     <numFmt numFmtId="167" formatCode="MM/DD/YY"/>
@@ -1215,26 +1220,26 @@
   </sheetPr>
   <dimension ref="A1:T5"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.1417004048583"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="33.5910931174089"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="14.6963562753036"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="6.97570850202429"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="12.9595141700405"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.2834008097166"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="9.91902834008097"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="14.5384615384615"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="8.71255060728745"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="6.45748987854251"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="12.9109311740891"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="8.1336032388664"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="14.7975708502024"/>
-    <col collapsed="false" hidden="false" max="1025" min="14" style="0" width="9.1417004048583"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="37.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="18.19"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="7.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="14.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="11.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="9.92"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="14.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="8.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="6.46"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="12.91"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="8.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="14.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="14" style="0" width="9.14"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="39.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1466,7 +1471,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -1481,20 +1486,20 @@
   </sheetPr>
   <dimension ref="A1:G35"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="7" width="18.668016194332"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="7" width="4.65587044534413"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="8" width="10.9109311740891"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="7" width="20.7085020242915"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="9" width="20.2226720647773"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="10" width="7.26315789473684"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="9" width="30.2307692307692"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.54251012145749"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="7" width="18.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="7" width="4.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="8" width="10.91"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="7" width="20.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="9" width="20.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="10" width="7.26"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="9" width="30.23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="8" style="0" width="8.54"/>
   </cols>
   <sheetData>
     <row r="1" s="14" customFormat="true" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2025,7 +2030,7 @@
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -2040,20 +2045,20 @@
   </sheetPr>
   <dimension ref="A1:G75"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A49" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A49" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A62" activeCellId="0" sqref="A62"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="7" width="27.8785425101215"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="22" width="5.16194331983806"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="8" width="10.3279352226721"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="7" width="17.5546558704453"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="9" width="27.8785425101215"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="8" width="7.22672064777328"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="9" width="30.9797570850202"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.54251012145749"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="7" width="27.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="22" width="5.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="8" width="10.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="7" width="17.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="9" width="27.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="8" width="7.23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="9" width="30.98"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="8" style="0" width="8.54"/>
   </cols>
   <sheetData>
     <row r="1" s="14" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3368,7 +3373,7 @@
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="5" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="5" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -3381,22 +3386,22 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G65536"/>
+  <dimension ref="A1:G1048576"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A37" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A37" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A36" activeCellId="0" sqref="A36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="7" width="27.8785425101215"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="22" width="5.16194331983806"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="8" width="10.3279352226721"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="7" width="17.5546558704453"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="9" width="27.8785425101215"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="8" width="7.22672064777328"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="9" width="30.9797570850202"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.54251012145749"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="7" width="27.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="22" width="5.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="8" width="10.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="7" width="17.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="9" width="27.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="8" width="7.23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="9" width="30.98"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="8" style="0" width="8.54"/>
   </cols>
   <sheetData>
     <row r="1" s="14" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4621,7 +4626,7 @@
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="5" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="5" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -4636,19 +4641,19 @@
   </sheetPr>
   <dimension ref="A1:G35"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A14" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A14" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E28" activeCellId="0" sqref="E28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.1619433198381"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="9.1417004048583"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.2672064777328"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="18.0526315789474"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="9.1417004048583"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="32.5425101214575"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="9.1417004048583"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="16.27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="18.05"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="32.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="8" style="0" width="9.14"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5153,7 +5158,7 @@
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>